<commit_message>
feat: Changes the combined_network attribute to be not visible
</commit_message>
<xml_diff>
--- a/sample-data/BBMRI-ERIC_model.xlsx
+++ b/sample-data/BBMRI-ERIC_model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\CRS4\Progetti\BBMRI\CS-IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A67A99D-C53A-41C7-A76E-ED02F7ED2EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3A0226-A275-43D8-802E-361BD022C057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28200" windowHeight="13935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1669,11 +1669,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1711,13 +1718,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4446,8 +4454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AO243"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11646,7 +11654,7 @@
       <c r="J102" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K102" s="2" t="s">
+      <c r="K102" s="6" t="s">
         <v>33</v>
       </c>
       <c r="L102" s="2" t="s">
@@ -11791,7 +11799,7 @@
         <v>33</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>33</v>

</xml_diff>